<commit_message>
Updated the documentation with the old runs that I completed.
</commit_message>
<xml_diff>
--- a/HW4/StatisticalAnalysis.xlsx
+++ b/HW4/StatisticalAnalysis.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UAH\CPE_512_Into_to_Parallel_Programming\HW4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krray\OneDrive\Documents\GitHub\CPE_512_Into_to_Parallel_Programming\HW4\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="20" documentId="9109FF9E7CA1D6D52444FC6660B835E50DB917E0" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{8FC16B82-7AD3-4DC6-8415-13379F8C3218}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="19">
   <si>
     <t>NP = 2</t>
   </si>
@@ -76,9 +77,6 @@
   </si>
   <si>
     <t>32/4</t>
-  </si>
-  <si>
-    <t>16/8</t>
   </si>
   <si>
     <t>Action 1.5</t>
@@ -483,13 +481,13 @@
       <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -506,7 +504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -523,7 +521,7 @@
         <v>32.537410999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -540,7 +538,7 @@
         <v>26.131996999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -557,7 +555,7 @@
         <v>22.022348999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -574,7 +572,7 @@
         <v>38.511263999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -591,7 +589,7 @@
         <v>51.449970999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -621,25 +619,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B80B94A-930A-4214-874A-1EF9F833C0A6}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -671,7 +669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -706,7 +704,7 @@
         <v>9.4904379999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -738,7 +736,7 @@
         <v>11.505651</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -770,7 +768,7 @@
         <v>9.4520739999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -802,7 +800,7 @@
         <v>9.8357209999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -834,7 +832,7 @@
         <v>9.8281379999999992</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -871,7 +869,7 @@
         <v>10.022404399999999</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -882,13 +880,25 @@
         <v>15</v>
       </c>
       <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s">
         <v>18</v>
       </c>
-      <c r="M9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
@@ -896,56 +906,127 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3">
+        <v>209.35736700000001</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3">
+        <v>10.51169</v>
+      </c>
       <c r="G12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="3">
-        <v>9.5190479999999997</v>
-      </c>
-      <c r="I12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10.170871</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <v>201.06361200000001</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3">
+        <v>9.6477319999999995</v>
+      </c>
       <c r="G13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H13" s="3">
-        <v>10.210634000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>9.3651929999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3">
+        <v>215.540524</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3">
+        <v>10.839015</v>
+      </c>
       <c r="G14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H14" s="3">
-        <v>8.5113979999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10.568781</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3">
+        <v>214.03624300000001</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3">
+        <v>10.424659999999999</v>
+      </c>
       <c r="G15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="3">
-        <v>8.7167209999999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10.236471</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3">
+        <v>215.44611499999999</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3">
+        <v>9.5849729999999997</v>
+      </c>
       <c r="G16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="3">
-        <v>8.4691790000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+        <v>9.4068769999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="7">
+        <f>AVERAGE(B12:B16)</f>
+        <v>211.08877219999999</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="7">
+        <f>AVERAGE(E12:E16)</f>
+        <v>10.201613999999999</v>
+      </c>
       <c r="G17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="7">
         <f>AVERAGE(H12:H16)</f>
-        <v>9.0853959999999994</v>
+        <v>9.9496386000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project Initialization.  The project is solution is up and the hashing functions are working, just need to implement the parallel part now.
</commit_message>
<xml_diff>
--- a/HW4/StatisticalAnalysis.xlsx
+++ b/HW4/StatisticalAnalysis.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krray\OneDrive\Documents\GitHub\CPE_512_Into_to_Parallel_Programming\HW4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UAH\CPE_512_Into_to_Parallel_Programming\HW4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="9109FF9E7CA1D6D52444FC6660B835E50DB917E0" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{B4BFB6AB-1B68-44C4-8DDF-D5467FE2C721}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="33">
   <si>
     <t>NP = 2</t>
   </si>
@@ -86,12 +85,54 @@
   </si>
   <si>
     <t>Action 1.7</t>
+  </si>
+  <si>
+    <t>Matrix Multiplication</t>
+  </si>
+  <si>
+    <t>Matrix Size</t>
+  </si>
+  <si>
+    <t>Action 2.1</t>
+  </si>
+  <si>
+    <t>Action 2.2</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Test 4</t>
+  </si>
+  <si>
+    <t>MPI NT = 2</t>
+  </si>
+  <si>
+    <t>MPI NT = 4</t>
+  </si>
+  <si>
+    <t>MPI NT = 8</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>Serial (s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -155,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -164,6 +205,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,13 +526,13 @@
       <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -507,7 +549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -524,7 +566,7 @@
         <v>32.537410999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -541,7 +583,7 @@
         <v>26.131996999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -558,7 +600,7 @@
         <v>22.022348999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -575,7 +617,7 @@
         <v>38.511263999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -592,7 +634,7 @@
         <v>51.449970999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -620,29 +662,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B80B94A-930A-4214-874A-1EF9F833C0A6}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11:U12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -673,8 +723,38 @@
       <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -708,8 +788,38 @@
       <c r="N2" s="3">
         <v>9.4904379999999993</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" s="2">
+        <v>8000</v>
+      </c>
+      <c r="U2" s="3">
+        <v>15.85561</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" s="2">
+        <v>512</v>
+      </c>
+      <c r="Y2" s="8">
+        <v>0.81897299999999995</v>
+      </c>
+      <c r="Z2" s="8">
+        <v>0.33041406000000001</v>
+      </c>
+      <c r="AA2" s="8">
+        <v>0.15570617</v>
+      </c>
+      <c r="AB2" s="8">
+        <v>8.0531835999999996E-2</v>
+      </c>
+      <c r="AC2" s="8">
+        <v>5.2849560000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -740,8 +850,38 @@
       <c r="N3" s="3">
         <v>11.505651</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" s="2">
+        <v>8000</v>
+      </c>
+      <c r="U3" s="3">
+        <v>18.199034999999999</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X3" s="2">
+        <v>1024</v>
+      </c>
+      <c r="Y3" s="8">
+        <v>6.7494370000000004</v>
+      </c>
+      <c r="Z3" s="8">
+        <v>3.3520522000000001</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>2.4545537999999998</v>
+      </c>
+      <c r="AB3" s="8">
+        <v>1.2403200000000001</v>
+      </c>
+      <c r="AC3" s="8">
+        <v>5.981198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -772,8 +912,38 @@
       <c r="N4" s="3">
         <v>9.4520739999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T4" s="2">
+        <v>8000</v>
+      </c>
+      <c r="U4" s="3">
+        <v>20.671267</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="2">
+        <v>2048</v>
+      </c>
+      <c r="Y4" s="8">
+        <v>91.993643000000006</v>
+      </c>
+      <c r="Z4" s="8">
+        <v>20.461957000000002</v>
+      </c>
+      <c r="AA4" s="8">
+        <v>12.809570000000001</v>
+      </c>
+      <c r="AB4" s="8">
+        <v>7.6243701000000001</v>
+      </c>
+      <c r="AC4" s="8">
+        <v>6.0197919999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -804,8 +974,38 @@
       <c r="N5" s="3">
         <v>9.8357209999999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="U5" s="3">
+        <v>14.721847</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X5" s="2">
+        <v>4096</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>1294.3027</v>
+      </c>
+      <c r="Z5" s="8">
+        <v>435.23511999999999</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>337.03656999999998</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>205.82470000000001</v>
+      </c>
+      <c r="AC5" s="8">
+        <v>7.5659419999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -836,8 +1036,17 @@
       <c r="N6" s="3">
         <v>9.8281379999999992</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T6" s="2">
+        <v>8000</v>
+      </c>
+      <c r="U6" s="3">
+        <v>15.835129999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -873,8 +1082,16 @@
         <f>AVERAGE(N2:N6)</f>
         <v>10.022404399999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T7" s="6"/>
+      <c r="U7" s="7">
+        <f>AVERAGE(U2:U6)</f>
+        <v>17.056577800000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -893,8 +1110,14 @@
       <c r="P9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S9" t="s">
+        <v>22</v>
+      </c>
+      <c r="W9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -931,8 +1154,17 @@
       <c r="Q11" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -969,8 +1201,17 @@
       <c r="Q12" s="3">
         <v>10.094671999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T12" s="2">
+        <v>8000</v>
+      </c>
+      <c r="U12" s="3">
+        <v>6481.8289000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1008,7 +1249,7 @@
         <v>9.2660230000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -1046,7 +1287,7 @@
         <v>10.277464999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1084,7 +1325,7 @@
         <v>6.1577060000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1122,7 +1363,7 @@
         <v>7.5581969999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -1168,5 +1409,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>